<commit_message>
fix synthesized strand file
</commit_message>
<xml_diff>
--- a/encoded-data/synthesized-strands.xlsx
+++ b/encoded-data/synthesized-strands.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
+    <t xml:space="preserve">HEDGES Design and Strand Names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplementary Table Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strand</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1/6) 1667 Encoding Full Length (Part of same image Thumbnail)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEDGES Index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplementary Table Index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strand</t>
   </si>
   <si>
     <t xml:space="preserve">(204, 13, 0)</t>
@@ -328,38 +328,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB30"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="78.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="196.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -386,292 +383,324 @@
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="B7" s="5" t="n">
-        <v>18</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B10" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B12" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B13" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9"/>
-    </row>
-    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B16" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B17" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="9"/>
     </row>
-    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="5" t="n">
+      <c r="B21" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="8" t="n">
+      <c r="B22" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="5" t="n">
+      <c r="B26" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="8" t="n">
+      <c r="B27" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="1"/>
-    </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="A28" s="1"/>
       <c r="B28" s="6"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="5" t="n">
+      <c r="B30" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="8" t="n">
+      <c r="B31" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>